<commit_message>
Update contingency tables with NA values removed
</commit_message>
<xml_diff>
--- a/Unique_analysis/proportion_calculations_unique.xlsx
+++ b/Unique_analysis/proportion_calculations_unique.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanso\OneDrive\Documents\Extreme Events\Unique_analysis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10980" windowHeight="3240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23140" windowHeight="13880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="proportion_calculations.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>&lt;1 sq m</t>
   </si>
@@ -150,19 +145,45 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Before+After</t>
+  </si>
+  <si>
+    <t>Before+During</t>
+  </si>
+  <si>
+    <t>Before+During+After</t>
+  </si>
+  <si>
+    <t>During</t>
+  </si>
+  <si>
+    <t>During+After</t>
+  </si>
+  <si>
+    <t>Duration Category</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Proportion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -181,6 +202,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -315,6 +344,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -387,7 +457,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,18 +502,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -851,30 +926,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="2"/>
@@ -898,7 +973,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -925,7 +1000,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -946,7 +1021,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -967,7 +1042,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -988,7 +1063,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +1084,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1105,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
@@ -1051,17 +1126,17 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2"/>
@@ -1085,7 +1160,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1185,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1131,7 +1206,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1152,7 +1227,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1173,7 +1248,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -1194,7 +1269,7 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1290,7 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1236,20 +1311,20 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
       <c r="J21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
@@ -1274,7 +1349,7 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="25"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -1295,7 +1370,7 @@
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="25"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1394,7 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="25"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="3" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1419,7 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="25"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1365,7 +1440,7 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="25"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="3" t="s">
         <v>16</v>
       </c>
@@ -1389,7 +1464,7 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="25"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="10" t="s">
         <v>17</v>
       </c>
@@ -1414,14 +1489,14 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:10">
       <c r="B31" s="2"/>
@@ -1445,7 +1520,7 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1472,7 +1547,7 @@
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="25"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
@@ -1493,7 +1568,7 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="25"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="3" t="s">
         <v>15</v>
       </c>
@@ -1517,7 +1592,7 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="25"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
@@ -1542,7 +1617,7 @@
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="25"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
@@ -1563,7 +1638,7 @@
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="25"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
@@ -1587,7 +1662,7 @@
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="25"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="10" t="s">
         <v>17</v>
       </c>
@@ -1612,14 +1687,14 @@
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:10">
       <c r="B41" s="2"/>
@@ -1643,7 +1718,7 @@
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -1670,7 +1745,7 @@
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="25"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="3" t="s">
         <v>15</v>
       </c>
@@ -1691,7 +1766,7 @@
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="25"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="3" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1790,7 @@
       </c>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="25"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="3" t="s">
         <v>19</v>
       </c>
@@ -1740,7 +1815,7 @@
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="25"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="3" t="s">
         <v>16</v>
       </c>
@@ -1761,7 +1836,7 @@
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="25"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="10" t="s">
         <v>17</v>
       </c>
@@ -1785,13 +1860,13 @@
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="25"/>
+      <c r="A48" s="22"/>
       <c r="J48">
         <f>C45+D45+E45+F45+G45</f>
         <v>6.1224489795918297E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="63">
+    <row r="50" spans="1:5" ht="60">
       <c r="A50" s="1"/>
       <c r="B50" s="13" t="s">
         <v>37</v>
@@ -1887,21 +1962,98 @@
         <v>6.1224489795918297E-2</v>
       </c>
     </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="27">
+        <v>3</v>
+      </c>
+      <c r="C60" s="5">
+        <v>5.6603773584905703E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="27">
+        <v>7</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0.13207547169811301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="27">
+        <v>5</v>
+      </c>
+      <c r="C62" s="5">
+        <v>9.4339622641509399E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="27">
+        <v>26</v>
+      </c>
+      <c r="C63" s="5">
+        <v>0.490566037735849</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" s="27">
+        <v>4</v>
+      </c>
+      <c r="C64" s="5">
+        <v>7.5471698113207503E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" s="28">
+        <v>8</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.15094339622641501</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A22:A28"/>
     <mergeCell ref="A32:A38"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="A42:A48"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A22:A28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>